<commit_message>
Add documentation to nps_create_master_df.py
</commit_message>
<xml_diff>
--- a/df_master.xlsx
+++ b/df_master.xlsx
@@ -931,7 +931,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>National Recreation Area</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -4609,7 +4609,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Park</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
@@ -6379,7 +6379,7 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Park</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
@@ -9179,7 +9179,7 @@
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>National Historic Site</t>
         </is>
       </c>
       <c r="E154" t="inlineStr">
@@ -9435,7 +9435,7 @@
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Park</t>
         </is>
       </c>
       <c r="E158" t="inlineStr">
@@ -12571,7 +12571,7 @@
       </c>
       <c r="D209" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Scenic &amp; Recreational River</t>
         </is>
       </c>
       <c r="E209" t="inlineStr">
@@ -12785,7 +12785,7 @@
       </c>
       <c r="D213" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>National Historic Landmark District</t>
         </is>
       </c>
       <c r="E213" t="inlineStr">
@@ -13381,7 +13381,7 @@
       </c>
       <c r="D223" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Park</t>
         </is>
       </c>
       <c r="E223" t="inlineStr">
@@ -14451,7 +14451,7 @@
       </c>
       <c r="D242" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Heritage Center</t>
         </is>
       </c>
       <c r="E242" t="inlineStr">
@@ -15759,7 +15759,7 @@
       </c>
       <c r="D265" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Park</t>
         </is>
       </c>
       <c r="E265" t="inlineStr">
@@ -19523,7 +19523,7 @@
       </c>
       <c r="D329" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Park</t>
         </is>
       </c>
       <c r="E329" t="inlineStr">
@@ -19587,7 +19587,7 @@
       </c>
       <c r="D330" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Park</t>
         </is>
       </c>
       <c r="E330" t="inlineStr">
@@ -19715,7 +19715,7 @@
       </c>
       <c r="D332" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Park</t>
         </is>
       </c>
       <c r="E332" t="inlineStr">
@@ -21147,7 +21147,7 @@
       </c>
       <c r="D358" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Park</t>
         </is>
       </c>
       <c r="E358" t="inlineStr">
@@ -21615,7 +21615,7 @@
       </c>
       <c r="D366" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Park</t>
         </is>
       </c>
       <c r="E366" t="inlineStr">
@@ -22569,7 +22569,7 @@
       </c>
       <c r="D382" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Park</t>
         </is>
       </c>
       <c r="E382" t="inlineStr">
@@ -26747,7 +26747,7 @@
       </c>
       <c r="D453" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>National Monument</t>
         </is>
       </c>
       <c r="E453" t="inlineStr">
@@ -28617,7 +28617,7 @@
       </c>
       <c r="D485" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Park</t>
         </is>
       </c>
       <c r="E485" t="inlineStr">

</xml_diff>